<commit_message>
Invoice temp changed By Richard 20160613
</commit_message>
<xml_diff>
--- a/02_Management/OZTT_Invoice_template.xlsx
+++ b/02_Management/OZTT_Invoice_template.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MyGitHub\OZTT-2016\02_Management\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="135" windowWidth="19395" windowHeight="7605"/>
+    <workbookView xWindow="600" yWindow="132" windowWidth="19392" windowHeight="7608"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
@@ -17,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="56">
   <si>
     <t>Code</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -212,14 +217,42 @@
   </si>
   <si>
     <t>LOGO区域</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>address：XXXXXXXXXXXXXXXXXXXXXXXXXXXXXXX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>address：地址</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>个人名称/公司名称：</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>公司abn：</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Email：</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>地址：</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name：个人名称/公司名称+空格+公司abn</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -266,6 +299,14 @@
       <i/>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
@@ -413,7 +454,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -452,33 +493,63 @@
     </xf>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -489,6 +560,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -537,7 +611,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -570,9 +644,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -605,6 +696,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -781,16 +889,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:AO36"/>
+  <dimension ref="B2:BK36"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="2.6640625" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="2.625" style="2"/>
+    <col min="1" max="16384" width="2.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:41" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:63" x14ac:dyDescent="0.25">
       <c r="AC2" s="3"/>
       <c r="AD2" s="4"/>
       <c r="AE2" s="4"/>
@@ -805,7 +913,7 @@
       <c r="AN2" s="4"/>
       <c r="AO2" s="5"/>
     </row>
-    <row r="3" spans="2:41" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:63" x14ac:dyDescent="0.25">
       <c r="AC3" s="6"/>
       <c r="AD3" s="7"/>
       <c r="AE3" s="7"/>
@@ -820,7 +928,7 @@
       <c r="AN3" s="7"/>
       <c r="AO3" s="8"/>
     </row>
-    <row r="4" spans="2:41" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:63" x14ac:dyDescent="0.25">
       <c r="AC4" s="6"/>
       <c r="AD4" s="7"/>
       <c r="AE4" s="7"/>
@@ -837,7 +945,7 @@
       <c r="AN4" s="7"/>
       <c r="AO4" s="8"/>
     </row>
-    <row r="5" spans="2:41" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:63" x14ac:dyDescent="0.25">
       <c r="AC5" s="6"/>
       <c r="AD5" s="7"/>
       <c r="AE5" s="7"/>
@@ -852,7 +960,7 @@
       <c r="AN5" s="7"/>
       <c r="AO5" s="8"/>
     </row>
-    <row r="6" spans="2:41" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:63" x14ac:dyDescent="0.25">
       <c r="AC6" s="6"/>
       <c r="AD6" s="7"/>
       <c r="AE6" s="7"/>
@@ -867,7 +975,7 @@
       <c r="AN6" s="7"/>
       <c r="AO6" s="8"/>
     </row>
-    <row r="7" spans="2:41" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:63" x14ac:dyDescent="0.25">
       <c r="AC7" s="10"/>
       <c r="AD7" s="11"/>
       <c r="AE7" s="11"/>
@@ -882,7 +990,7 @@
       <c r="AN7" s="11"/>
       <c r="AO7" s="12"/>
     </row>
-    <row r="8" spans="2:41" x14ac:dyDescent="0.15">
+    <row r="8" spans="2:63" x14ac:dyDescent="0.25">
       <c r="AC8" s="7"/>
       <c r="AD8" s="7"/>
       <c r="AE8" s="7"/>
@@ -897,19 +1005,19 @@
       <c r="AN8" s="7"/>
       <c r="AO8" s="7"/>
     </row>
-    <row r="9" spans="2:41" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="R9" s="20" t="s">
+    <row r="9" spans="2:63" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R9" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="S9" s="20"/>
-      <c r="T9" s="20"/>
-      <c r="U9" s="20"/>
-      <c r="V9" s="20"/>
-      <c r="W9" s="20"/>
-      <c r="X9" s="20"/>
-      <c r="Y9" s="20"/>
-    </row>
-    <row r="13" spans="2:41" x14ac:dyDescent="0.15">
+      <c r="S9" s="13"/>
+      <c r="T9" s="13"/>
+      <c r="U9" s="13"/>
+      <c r="V9" s="13"/>
+      <c r="W9" s="13"/>
+      <c r="X9" s="13"/>
+      <c r="Y9" s="13"/>
+    </row>
+    <row r="13" spans="2:63" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>5</v>
       </c>
@@ -917,63 +1025,128 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="2:41" x14ac:dyDescent="0.15">
+    <row r="14" spans="2:63" x14ac:dyDescent="0.25">
       <c r="W14" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="15" spans="2:41" x14ac:dyDescent="0.15">
-      <c r="C15" s="3" t="s">
+      <c r="AQ14" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="AR14" s="28"/>
+      <c r="AS14" s="28"/>
+      <c r="AT14" s="28"/>
+      <c r="AU14" s="28"/>
+      <c r="AV14" s="28"/>
+      <c r="AW14" s="28"/>
+      <c r="AX14" s="28"/>
+      <c r="AY14" s="28"/>
+      <c r="AZ14" s="28"/>
+      <c r="BA14" s="28"/>
+      <c r="BB14" s="28"/>
+      <c r="BC14" s="28"/>
+      <c r="BD14" s="28"/>
+      <c r="BE14" s="28"/>
+      <c r="BF14" s="28"/>
+      <c r="BG14" s="28"/>
+      <c r="BH14" s="28"/>
+      <c r="BI14" s="28"/>
+      <c r="BJ14" s="28"/>
+      <c r="BK14" s="28"/>
+    </row>
+    <row r="15" spans="2:63" x14ac:dyDescent="0.25">
+      <c r="C15" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4" t="s">
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
-      <c r="P15" s="4"/>
-      <c r="Q15" s="4"/>
-      <c r="R15" s="5"/>
-    </row>
-    <row r="16" spans="2:41" x14ac:dyDescent="0.15">
-      <c r="C16" s="6"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="7"/>
-      <c r="O16" s="7"/>
-      <c r="P16" s="7"/>
-      <c r="Q16" s="7"/>
-      <c r="R16" s="8"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="23"/>
+      <c r="M15" s="23"/>
+      <c r="N15" s="23"/>
+      <c r="O15" s="23"/>
+      <c r="P15" s="23"/>
+      <c r="Q15" s="23"/>
+      <c r="R15" s="24"/>
+      <c r="AQ15" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="AR15" s="28"/>
+      <c r="AS15" s="28"/>
+      <c r="AT15" s="28"/>
+      <c r="AU15" s="28"/>
+      <c r="AV15" s="28"/>
+      <c r="AW15" s="28"/>
+      <c r="AX15" s="28"/>
+      <c r="AY15" s="28"/>
+      <c r="AZ15" s="28"/>
+      <c r="BA15" s="28"/>
+      <c r="BB15" s="28"/>
+      <c r="BC15" s="28"/>
+      <c r="BD15" s="28"/>
+      <c r="BE15" s="28"/>
+      <c r="BF15" s="28"/>
+      <c r="BG15" s="28"/>
+      <c r="BH15" s="28"/>
+      <c r="BI15" s="28"/>
+      <c r="BJ15" s="28"/>
+      <c r="BK15" s="28"/>
+    </row>
+    <row r="16" spans="2:63" x14ac:dyDescent="0.25">
+      <c r="C16" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="26"/>
+      <c r="L16" s="26"/>
+      <c r="M16" s="26"/>
+      <c r="N16" s="26"/>
+      <c r="O16" s="26"/>
+      <c r="P16" s="26"/>
+      <c r="Q16" s="26"/>
+      <c r="R16" s="27"/>
       <c r="V16" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="2:41" x14ac:dyDescent="0.15">
-      <c r="C17" s="6" t="s">
-        <v>7</v>
-      </c>
+      <c r="AQ16" s="28"/>
+      <c r="AR16" s="28"/>
+      <c r="AS16" s="28"/>
+      <c r="AT16" s="28"/>
+      <c r="AU16" s="28"/>
+      <c r="AV16" s="28"/>
+      <c r="AW16" s="28"/>
+      <c r="AX16" s="28"/>
+      <c r="AY16" s="28"/>
+      <c r="AZ16" s="28"/>
+      <c r="BA16" s="28"/>
+      <c r="BB16" s="28"/>
+      <c r="BC16" s="28"/>
+      <c r="BD16" s="28"/>
+      <c r="BE16" s="28"/>
+      <c r="BF16" s="28"/>
+      <c r="BG16" s="28"/>
+      <c r="BH16" s="28"/>
+      <c r="BI16" s="28"/>
+      <c r="BJ16" s="28"/>
+      <c r="BK16" s="28"/>
+    </row>
+    <row r="17" spans="2:63" x14ac:dyDescent="0.25">
+      <c r="C17" s="6"/>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
-      <c r="F17" s="9" t="s">
-        <v>20</v>
-      </c>
+      <c r="F17" s="7"/>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
@@ -989,12 +1162,37 @@
       <c r="W17" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="2:41" x14ac:dyDescent="0.15">
-      <c r="C18" s="6"/>
+      <c r="AQ17" s="28"/>
+      <c r="AR17" s="28"/>
+      <c r="AS17" s="28"/>
+      <c r="AT17" s="22"/>
+      <c r="AU17" s="23"/>
+      <c r="AV17" s="23"/>
+      <c r="AW17" s="23"/>
+      <c r="AX17" s="23"/>
+      <c r="AY17" s="23"/>
+      <c r="AZ17" s="23"/>
+      <c r="BA17" s="23"/>
+      <c r="BB17" s="23"/>
+      <c r="BC17" s="23"/>
+      <c r="BD17" s="23"/>
+      <c r="BE17" s="23"/>
+      <c r="BF17" s="23"/>
+      <c r="BG17" s="24"/>
+      <c r="BH17" s="28"/>
+      <c r="BI17" s="28"/>
+      <c r="BJ17" s="28"/>
+      <c r="BK17" s="28"/>
+    </row>
+    <row r="18" spans="2:63" x14ac:dyDescent="0.25">
+      <c r="C18" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
+      <c r="F18" s="9" t="s">
+        <v>20</v>
+      </c>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
@@ -1007,8 +1205,31 @@
       <c r="P18" s="7"/>
       <c r="Q18" s="7"/>
       <c r="R18" s="8"/>
-    </row>
-    <row r="19" spans="2:41" x14ac:dyDescent="0.15">
+      <c r="AQ18" s="28"/>
+      <c r="AR18" s="28"/>
+      <c r="AS18" s="28"/>
+      <c r="AT18" s="25"/>
+      <c r="AU18" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="AV18" s="26"/>
+      <c r="AW18" s="26"/>
+      <c r="AX18" s="26"/>
+      <c r="AY18" s="26"/>
+      <c r="AZ18" s="26"/>
+      <c r="BA18" s="26"/>
+      <c r="BB18" s="26"/>
+      <c r="BC18" s="26"/>
+      <c r="BD18" s="26"/>
+      <c r="BE18" s="26"/>
+      <c r="BF18" s="26"/>
+      <c r="BG18" s="27"/>
+      <c r="BH18" s="28"/>
+      <c r="BI18" s="28"/>
+      <c r="BJ18" s="28"/>
+      <c r="BK18" s="28"/>
+    </row>
+    <row r="19" spans="2:63" x14ac:dyDescent="0.25">
       <c r="C19" s="10" t="s">
         <v>8</v>
       </c>
@@ -1032,23 +1253,111 @@
       <c r="V19" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="20" spans="2:41" x14ac:dyDescent="0.15">
+      <c r="AQ19" s="28"/>
+      <c r="AR19" s="28"/>
+      <c r="AS19" s="28"/>
+      <c r="AT19" s="25"/>
+      <c r="AU19" s="26"/>
+      <c r="AV19" s="26"/>
+      <c r="AW19" s="26"/>
+      <c r="AX19" s="26"/>
+      <c r="AY19" s="26"/>
+      <c r="AZ19" s="26"/>
+      <c r="BA19" s="26"/>
+      <c r="BB19" s="26"/>
+      <c r="BC19" s="26"/>
+      <c r="BD19" s="26"/>
+      <c r="BE19" s="26"/>
+      <c r="BF19" s="26"/>
+      <c r="BG19" s="27"/>
+      <c r="BH19" s="28"/>
+      <c r="BI19" s="28"/>
+      <c r="BJ19" s="28"/>
+      <c r="BK19" s="28"/>
+    </row>
+    <row r="20" spans="2:63" x14ac:dyDescent="0.25">
       <c r="W20" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="21" spans="2:41" x14ac:dyDescent="0.15">
+      <c r="AQ20" s="28"/>
+      <c r="AR20" s="28"/>
+      <c r="AS20" s="28"/>
+      <c r="AT20" s="25"/>
+      <c r="AU20" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="AV20" s="26"/>
+      <c r="AW20" s="26"/>
+      <c r="AX20" s="26"/>
+      <c r="AY20" s="26"/>
+      <c r="AZ20" s="26"/>
+      <c r="BA20" s="26"/>
+      <c r="BB20" s="26"/>
+      <c r="BC20" s="26"/>
+      <c r="BD20" s="26"/>
+      <c r="BE20" s="26"/>
+      <c r="BF20" s="26"/>
+      <c r="BG20" s="27"/>
+      <c r="BH20" s="28"/>
+      <c r="BI20" s="28"/>
+      <c r="BJ20" s="28"/>
+      <c r="BK20" s="28"/>
+    </row>
+    <row r="21" spans="2:63" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="22" spans="2:41" x14ac:dyDescent="0.15">
+      <c r="AQ21" s="28"/>
+      <c r="AR21" s="28"/>
+      <c r="AS21" s="28"/>
+      <c r="AT21" s="25"/>
+      <c r="AU21" s="26"/>
+      <c r="AV21" s="26"/>
+      <c r="AW21" s="26"/>
+      <c r="AX21" s="26"/>
+      <c r="AY21" s="26"/>
+      <c r="AZ21" s="26"/>
+      <c r="BA21" s="26"/>
+      <c r="BB21" s="26"/>
+      <c r="BC21" s="26"/>
+      <c r="BD21" s="26"/>
+      <c r="BE21" s="26"/>
+      <c r="BF21" s="26"/>
+      <c r="BG21" s="27"/>
+      <c r="BH21" s="28"/>
+      <c r="BI21" s="28"/>
+      <c r="BJ21" s="28"/>
+      <c r="BK21" s="28"/>
+    </row>
+    <row r="22" spans="2:63" x14ac:dyDescent="0.25">
       <c r="V22" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="23" spans="2:41" x14ac:dyDescent="0.15">
+      <c r="AQ22" s="28"/>
+      <c r="AR22" s="28"/>
+      <c r="AS22" s="28"/>
+      <c r="AT22" s="25"/>
+      <c r="AU22" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="AV22" s="26"/>
+      <c r="AW22" s="26"/>
+      <c r="AX22" s="26"/>
+      <c r="AY22" s="26"/>
+      <c r="AZ22" s="26"/>
+      <c r="BA22" s="26"/>
+      <c r="BB22" s="26"/>
+      <c r="BC22" s="26"/>
+      <c r="BD22" s="26"/>
+      <c r="BE22" s="26"/>
+      <c r="BF22" s="26"/>
+      <c r="BG22" s="27"/>
+      <c r="BH22" s="28"/>
+      <c r="BI22" s="28"/>
+      <c r="BJ22" s="28"/>
+      <c r="BK22" s="28"/>
+    </row>
+    <row r="23" spans="2:63" x14ac:dyDescent="0.25">
       <c r="C23" s="3" t="s">
         <v>22</v>
       </c>
@@ -1070,8 +1379,29 @@
       <c r="W23" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="24" spans="2:41" x14ac:dyDescent="0.15">
+      <c r="AQ23" s="28"/>
+      <c r="AR23" s="28"/>
+      <c r="AS23" s="28"/>
+      <c r="AT23" s="25"/>
+      <c r="AU23" s="26"/>
+      <c r="AV23" s="26"/>
+      <c r="AW23" s="26"/>
+      <c r="AX23" s="26"/>
+      <c r="AY23" s="26"/>
+      <c r="AZ23" s="26"/>
+      <c r="BA23" s="26"/>
+      <c r="BB23" s="26"/>
+      <c r="BC23" s="26"/>
+      <c r="BD23" s="26"/>
+      <c r="BE23" s="26"/>
+      <c r="BF23" s="26"/>
+      <c r="BG23" s="27"/>
+      <c r="BH23" s="28"/>
+      <c r="BI23" s="28"/>
+      <c r="BJ23" s="28"/>
+      <c r="BK23" s="28"/>
+    </row>
+    <row r="24" spans="2:63" x14ac:dyDescent="0.25">
       <c r="C24" s="6" t="s">
         <v>23</v>
       </c>
@@ -1090,8 +1420,31 @@
       <c r="P24" s="7"/>
       <c r="Q24" s="7"/>
       <c r="R24" s="8"/>
-    </row>
-    <row r="25" spans="2:41" x14ac:dyDescent="0.15">
+      <c r="AQ24" s="28"/>
+      <c r="AR24" s="28"/>
+      <c r="AS24" s="28"/>
+      <c r="AT24" s="25"/>
+      <c r="AU24" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="AV24" s="26"/>
+      <c r="AW24" s="26"/>
+      <c r="AX24" s="26"/>
+      <c r="AY24" s="26"/>
+      <c r="AZ24" s="26"/>
+      <c r="BA24" s="26"/>
+      <c r="BB24" s="26"/>
+      <c r="BC24" s="26"/>
+      <c r="BD24" s="26"/>
+      <c r="BE24" s="26"/>
+      <c r="BF24" s="26"/>
+      <c r="BG24" s="27"/>
+      <c r="BH24" s="28"/>
+      <c r="BI24" s="28"/>
+      <c r="BJ24" s="28"/>
+      <c r="BK24" s="28"/>
+    </row>
+    <row r="25" spans="2:63" x14ac:dyDescent="0.25">
       <c r="C25" s="6" t="s">
         <v>24</v>
       </c>
@@ -1113,8 +1466,29 @@
       <c r="V25" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="26" spans="2:41" x14ac:dyDescent="0.15">
+      <c r="AQ25" s="28"/>
+      <c r="AR25" s="28"/>
+      <c r="AS25" s="28"/>
+      <c r="AT25" s="29"/>
+      <c r="AU25" s="30"/>
+      <c r="AV25" s="30"/>
+      <c r="AW25" s="30"/>
+      <c r="AX25" s="30"/>
+      <c r="AY25" s="30"/>
+      <c r="AZ25" s="30"/>
+      <c r="BA25" s="30"/>
+      <c r="BB25" s="30"/>
+      <c r="BC25" s="30"/>
+      <c r="BD25" s="30"/>
+      <c r="BE25" s="30"/>
+      <c r="BF25" s="30"/>
+      <c r="BG25" s="31"/>
+      <c r="BH25" s="28"/>
+      <c r="BI25" s="28"/>
+      <c r="BJ25" s="28"/>
+      <c r="BK25" s="28"/>
+    </row>
+    <row r="26" spans="2:63" x14ac:dyDescent="0.25">
       <c r="C26" s="10" t="s">
         <v>25</v>
       </c>
@@ -1137,7 +1511,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="2:41" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="2:63" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="21" t="s">
         <v>0</v>
       </c>
@@ -1191,244 +1565,268 @@
       <c r="AN29" s="21"/>
       <c r="AO29" s="21"/>
     </row>
-    <row r="30" spans="2:41" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B30" s="13" t="s">
+    <row r="30" spans="2:63" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13" t="s">
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="H30" s="13"/>
-      <c r="I30" s="13"/>
-      <c r="J30" s="13"/>
-      <c r="K30" s="13"/>
-      <c r="L30" s="13"/>
-      <c r="M30" s="13"/>
-      <c r="N30" s="13"/>
-      <c r="O30" s="13"/>
-      <c r="P30" s="13"/>
-      <c r="Q30" s="13"/>
-      <c r="R30" s="13"/>
-      <c r="S30" s="13"/>
-      <c r="T30" s="13"/>
-      <c r="U30" s="13"/>
-      <c r="V30" s="15" t="s">
+      <c r="H30" s="19"/>
+      <c r="I30" s="19"/>
+      <c r="J30" s="19"/>
+      <c r="K30" s="19"/>
+      <c r="L30" s="19"/>
+      <c r="M30" s="19"/>
+      <c r="N30" s="19"/>
+      <c r="O30" s="19"/>
+      <c r="P30" s="19"/>
+      <c r="Q30" s="19"/>
+      <c r="R30" s="19"/>
+      <c r="S30" s="19"/>
+      <c r="T30" s="19"/>
+      <c r="U30" s="19"/>
+      <c r="V30" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="W30" s="15"/>
-      <c r="X30" s="15"/>
-      <c r="Y30" s="15"/>
-      <c r="Z30" s="15"/>
-      <c r="AA30" s="15" t="s">
+      <c r="W30" s="20"/>
+      <c r="X30" s="20"/>
+      <c r="Y30" s="20"/>
+      <c r="Z30" s="20"/>
+      <c r="AA30" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="AB30" s="15"/>
-      <c r="AC30" s="15"/>
-      <c r="AD30" s="15"/>
-      <c r="AE30" s="15"/>
-      <c r="AF30" s="15" t="s">
+      <c r="AB30" s="20"/>
+      <c r="AC30" s="20"/>
+      <c r="AD30" s="20"/>
+      <c r="AE30" s="20"/>
+      <c r="AF30" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="AG30" s="15"/>
-      <c r="AH30" s="15"/>
-      <c r="AI30" s="15"/>
-      <c r="AJ30" s="15"/>
-      <c r="AK30" s="15" t="s">
+      <c r="AG30" s="20"/>
+      <c r="AH30" s="20"/>
+      <c r="AI30" s="20"/>
+      <c r="AJ30" s="20"/>
+      <c r="AK30" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="AL30" s="15"/>
-      <c r="AM30" s="15"/>
-      <c r="AN30" s="15"/>
-      <c r="AO30" s="15"/>
-    </row>
-    <row r="31" spans="2:41" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B31" s="13" t="s">
+      <c r="AL30" s="20"/>
+      <c r="AM30" s="20"/>
+      <c r="AN30" s="20"/>
+      <c r="AO30" s="20"/>
+    </row>
+    <row r="31" spans="2:63" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13" t="s">
+      <c r="C31" s="19"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="H31" s="13"/>
-      <c r="I31" s="13"/>
-      <c r="J31" s="13"/>
-      <c r="K31" s="13"/>
-      <c r="L31" s="13"/>
-      <c r="M31" s="13"/>
-      <c r="N31" s="13"/>
-      <c r="O31" s="13"/>
-      <c r="P31" s="13"/>
-      <c r="Q31" s="13"/>
-      <c r="R31" s="13"/>
-      <c r="S31" s="13"/>
-      <c r="T31" s="13"/>
-      <c r="U31" s="13"/>
-      <c r="V31" s="15" t="s">
+      <c r="H31" s="19"/>
+      <c r="I31" s="19"/>
+      <c r="J31" s="19"/>
+      <c r="K31" s="19"/>
+      <c r="L31" s="19"/>
+      <c r="M31" s="19"/>
+      <c r="N31" s="19"/>
+      <c r="O31" s="19"/>
+      <c r="P31" s="19"/>
+      <c r="Q31" s="19"/>
+      <c r="R31" s="19"/>
+      <c r="S31" s="19"/>
+      <c r="T31" s="19"/>
+      <c r="U31" s="19"/>
+      <c r="V31" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="W31" s="15"/>
-      <c r="X31" s="15"/>
-      <c r="Y31" s="15"/>
-      <c r="Z31" s="15"/>
-      <c r="AA31" s="15" t="s">
+      <c r="W31" s="20"/>
+      <c r="X31" s="20"/>
+      <c r="Y31" s="20"/>
+      <c r="Z31" s="20"/>
+      <c r="AA31" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="AB31" s="15"/>
-      <c r="AC31" s="15"/>
-      <c r="AD31" s="15"/>
-      <c r="AE31" s="15"/>
-      <c r="AF31" s="15" t="s">
+      <c r="AB31" s="20"/>
+      <c r="AC31" s="20"/>
+      <c r="AD31" s="20"/>
+      <c r="AE31" s="20"/>
+      <c r="AF31" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="AG31" s="15"/>
-      <c r="AH31" s="15"/>
-      <c r="AI31" s="15"/>
-      <c r="AJ31" s="15"/>
-      <c r="AK31" s="15" t="s">
+      <c r="AG31" s="20"/>
+      <c r="AH31" s="20"/>
+      <c r="AI31" s="20"/>
+      <c r="AJ31" s="20"/>
+      <c r="AK31" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="AL31" s="15"/>
-      <c r="AM31" s="15"/>
-      <c r="AN31" s="15"/>
-      <c r="AO31" s="15"/>
-    </row>
-    <row r="32" spans="2:41" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B32" s="14" t="s">
+      <c r="AL31" s="20"/>
+      <c r="AM31" s="20"/>
+      <c r="AN31" s="20"/>
+      <c r="AO31" s="20"/>
+    </row>
+    <row r="32" spans="2:63" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14" t="s">
+      <c r="C32" s="17"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="H32" s="14"/>
-      <c r="I32" s="14"/>
-      <c r="J32" s="14"/>
-      <c r="K32" s="14"/>
-      <c r="L32" s="14"/>
-      <c r="M32" s="14"/>
-      <c r="N32" s="14"/>
-      <c r="O32" s="14"/>
-      <c r="P32" s="14"/>
-      <c r="Q32" s="14"/>
-      <c r="R32" s="14"/>
-      <c r="S32" s="14"/>
-      <c r="T32" s="14"/>
-      <c r="U32" s="14"/>
-      <c r="V32" s="16" t="s">
+      <c r="H32" s="17"/>
+      <c r="I32" s="17"/>
+      <c r="J32" s="17"/>
+      <c r="K32" s="17"/>
+      <c r="L32" s="17"/>
+      <c r="M32" s="17"/>
+      <c r="N32" s="17"/>
+      <c r="O32" s="17"/>
+      <c r="P32" s="17"/>
+      <c r="Q32" s="17"/>
+      <c r="R32" s="17"/>
+      <c r="S32" s="17"/>
+      <c r="T32" s="17"/>
+      <c r="U32" s="17"/>
+      <c r="V32" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="W32" s="16"/>
-      <c r="X32" s="16"/>
-      <c r="Y32" s="16"/>
-      <c r="Z32" s="16"/>
-      <c r="AA32" s="16" t="s">
+      <c r="W32" s="18"/>
+      <c r="X32" s="18"/>
+      <c r="Y32" s="18"/>
+      <c r="Z32" s="18"/>
+      <c r="AA32" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="AB32" s="16"/>
-      <c r="AC32" s="16"/>
-      <c r="AD32" s="16"/>
-      <c r="AE32" s="16"/>
-      <c r="AF32" s="16" t="s">
+      <c r="AB32" s="18"/>
+      <c r="AC32" s="18"/>
+      <c r="AD32" s="18"/>
+      <c r="AE32" s="18"/>
+      <c r="AF32" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="AG32" s="16"/>
-      <c r="AH32" s="16"/>
-      <c r="AI32" s="16"/>
-      <c r="AJ32" s="16"/>
-      <c r="AK32" s="16" t="s">
+      <c r="AG32" s="18"/>
+      <c r="AH32" s="18"/>
+      <c r="AI32" s="18"/>
+      <c r="AJ32" s="18"/>
+      <c r="AK32" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="AL32" s="16"/>
-      <c r="AM32" s="16"/>
-      <c r="AN32" s="16"/>
-      <c r="AO32" s="16"/>
-    </row>
-    <row r="33" spans="19:37" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="34" spans="19:37" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="S34" s="17" t="s">
+      <c r="AL32" s="18"/>
+      <c r="AM32" s="18"/>
+      <c r="AN32" s="18"/>
+      <c r="AO32" s="18"/>
+    </row>
+    <row r="33" spans="19:37" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="19:37" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S34" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="T34" s="17"/>
-      <c r="U34" s="17"/>
-      <c r="V34" s="17"/>
-      <c r="W34" s="17"/>
-      <c r="X34" s="17"/>
-      <c r="Y34" s="17"/>
-      <c r="Z34" s="17"/>
-      <c r="AA34" s="17"/>
-      <c r="AB34" s="17"/>
-      <c r="AC34" s="17"/>
-      <c r="AD34" s="17"/>
-      <c r="AE34" s="17"/>
-      <c r="AF34" s="17" t="s">
+      <c r="T34" s="14"/>
+      <c r="U34" s="14"/>
+      <c r="V34" s="14"/>
+      <c r="W34" s="14"/>
+      <c r="X34" s="14"/>
+      <c r="Y34" s="14"/>
+      <c r="Z34" s="14"/>
+      <c r="AA34" s="14"/>
+      <c r="AB34" s="14"/>
+      <c r="AC34" s="14"/>
+      <c r="AD34" s="14"/>
+      <c r="AE34" s="14"/>
+      <c r="AF34" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="AG34" s="17"/>
-      <c r="AH34" s="17"/>
-      <c r="AI34" s="17"/>
-      <c r="AJ34" s="17"/>
-    </row>
-    <row r="35" spans="19:37" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="S35" s="17" t="s">
+      <c r="AG34" s="14"/>
+      <c r="AH34" s="14"/>
+      <c r="AI34" s="14"/>
+      <c r="AJ34" s="14"/>
+    </row>
+    <row r="35" spans="19:37" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S35" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="T35" s="17"/>
-      <c r="U35" s="17"/>
-      <c r="V35" s="17"/>
-      <c r="W35" s="17"/>
-      <c r="X35" s="17"/>
-      <c r="Y35" s="17"/>
-      <c r="Z35" s="17"/>
-      <c r="AA35" s="17"/>
-      <c r="AB35" s="17"/>
-      <c r="AC35" s="17"/>
-      <c r="AD35" s="17"/>
-      <c r="AE35" s="17"/>
-      <c r="AF35" s="19" t="s">
+      <c r="T35" s="14"/>
+      <c r="U35" s="14"/>
+      <c r="V35" s="14"/>
+      <c r="W35" s="14"/>
+      <c r="X35" s="14"/>
+      <c r="Y35" s="14"/>
+      <c r="Z35" s="14"/>
+      <c r="AA35" s="14"/>
+      <c r="AB35" s="14"/>
+      <c r="AC35" s="14"/>
+      <c r="AD35" s="14"/>
+      <c r="AE35" s="14"/>
+      <c r="AF35" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="AG35" s="19"/>
-      <c r="AH35" s="19"/>
-      <c r="AI35" s="19"/>
-      <c r="AJ35" s="19"/>
-    </row>
-    <row r="36" spans="19:37" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="S36" s="18" t="s">
+      <c r="AG35" s="16"/>
+      <c r="AH35" s="16"/>
+      <c r="AI35" s="16"/>
+      <c r="AJ35" s="16"/>
+    </row>
+    <row r="36" spans="19:37" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S36" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="T36" s="18"/>
-      <c r="U36" s="18"/>
-      <c r="V36" s="18"/>
-      <c r="W36" s="18"/>
-      <c r="X36" s="18"/>
-      <c r="Y36" s="18"/>
-      <c r="Z36" s="18"/>
-      <c r="AA36" s="18"/>
-      <c r="AB36" s="18"/>
-      <c r="AC36" s="18"/>
-      <c r="AD36" s="18"/>
-      <c r="AE36" s="18"/>
-      <c r="AF36" s="18" t="s">
+      <c r="T36" s="15"/>
+      <c r="U36" s="15"/>
+      <c r="V36" s="15"/>
+      <c r="W36" s="15"/>
+      <c r="X36" s="15"/>
+      <c r="Y36" s="15"/>
+      <c r="Z36" s="15"/>
+      <c r="AA36" s="15"/>
+      <c r="AB36" s="15"/>
+      <c r="AC36" s="15"/>
+      <c r="AD36" s="15"/>
+      <c r="AE36" s="15"/>
+      <c r="AF36" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="AG36" s="18"/>
-      <c r="AH36" s="18"/>
-      <c r="AI36" s="18"/>
-      <c r="AJ36" s="18"/>
+      <c r="AG36" s="15"/>
+      <c r="AH36" s="15"/>
+      <c r="AI36" s="15"/>
+      <c r="AJ36" s="15"/>
       <c r="AK36" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="AK30:AO30"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="G29:U29"/>
+    <mergeCell ref="V29:Z29"/>
+    <mergeCell ref="AA29:AE29"/>
+    <mergeCell ref="AF29:AJ29"/>
+    <mergeCell ref="AK29:AO29"/>
+    <mergeCell ref="B30:F30"/>
+    <mergeCell ref="G30:U30"/>
+    <mergeCell ref="V30:Z30"/>
+    <mergeCell ref="AA30:AE30"/>
+    <mergeCell ref="AF30:AJ30"/>
+    <mergeCell ref="AK32:AO32"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="G31:U31"/>
+    <mergeCell ref="V31:Z31"/>
+    <mergeCell ref="AA31:AE31"/>
+    <mergeCell ref="AF31:AJ31"/>
+    <mergeCell ref="AK31:AO31"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="G32:U32"/>
+    <mergeCell ref="V32:Z32"/>
+    <mergeCell ref="AA32:AE32"/>
+    <mergeCell ref="AF32:AJ32"/>
     <mergeCell ref="R9:Y9"/>
     <mergeCell ref="S34:AE34"/>
     <mergeCell ref="S35:AE35"/>
@@ -1436,33 +1834,9 @@
     <mergeCell ref="AF34:AJ34"/>
     <mergeCell ref="AF35:AJ35"/>
     <mergeCell ref="AF36:AJ36"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="G32:U32"/>
-    <mergeCell ref="V32:Z32"/>
-    <mergeCell ref="AA32:AE32"/>
-    <mergeCell ref="AF32:AJ32"/>
-    <mergeCell ref="AK32:AO32"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="G31:U31"/>
-    <mergeCell ref="V31:Z31"/>
-    <mergeCell ref="AA31:AE31"/>
-    <mergeCell ref="AF31:AJ31"/>
-    <mergeCell ref="AK31:AO31"/>
-    <mergeCell ref="B30:F30"/>
-    <mergeCell ref="G30:U30"/>
-    <mergeCell ref="V30:Z30"/>
-    <mergeCell ref="AA30:AE30"/>
-    <mergeCell ref="AF30:AJ30"/>
-    <mergeCell ref="AK30:AO30"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="G29:U29"/>
-    <mergeCell ref="V29:Z29"/>
-    <mergeCell ref="AA29:AE29"/>
-    <mergeCell ref="AF29:AJ29"/>
-    <mergeCell ref="AK29:AO29"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="78" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="78" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>